<commit_message>
Update importTopics, importStudents, importLecturers and createTranscript
</commit_message>
<xml_diff>
--- a/public/uploads/topics.xlsx
+++ b/public/uploads/topics.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coder\manage-graduation-thesis-iuh-be\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vscode\manage-graduation-thesis-iuh-be\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16836822-D069-43EA-BC5D-E7B501C06DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15996" windowHeight="4836"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Đè tài TN" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,12 +33,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tri Pham Quang</author>
   </authors>
   <commentList>
-    <comment ref="H4" authorId="0" shapeId="0">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -886,7 +892,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1021,7 +1027,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1067,7 +1073,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1378,13 +1384,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA986"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="14">
-        <v>20001239</v>
+        <v>20011239</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>6</v>
@@ -1548,7 +1554,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="14">
-        <v>20001243</v>
+        <v>20011243</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>17</v>
@@ -1595,7 +1601,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="14">
-        <v>20001243</v>
+        <v>20011243</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
fix: topic, lecturer, lcterm, topic ,student
</commit_message>
<xml_diff>
--- a/public/uploads/topics.xlsx
+++ b/public/uploads/topics.xlsx
@@ -1,31 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vscode\manage-graduation-thesis-iuh-be\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\UploadExcelTes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16836822-D069-43EA-BC5D-E7B501C06DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15996" windowHeight="4836"/>
   </bookViews>
   <sheets>
     <sheet name="Đè tài TN" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Tri Pham Quang</author>
   </authors>
   <commentList>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="H4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -892,7 +886,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1027,7 +1021,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1073,7 +1067,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1384,13 +1378,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA986"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1507,7 +1501,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="14">
-        <v>20001239</v>
+        <v>20011239</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -1554,7 +1548,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="14">
-        <v>20011243</v>
+        <v>20001243</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>17</v>
@@ -1601,7 +1595,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="14">
-        <v>20011243</v>
+        <v>20001243</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>17</v>
@@ -1837,7 +1831,7 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="1:27" ht="193.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="179.4" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -1983,7 +1977,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="14">
-        <v>20001255</v>
+        <v>21084321</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>130</v>
@@ -2030,7 +2024,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="14">
-        <v>20001255</v>
+        <v>21084321</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>128</v>
@@ -2077,7 +2071,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="14">
-        <v>20001255</v>
+        <v>21084321</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>128</v>
@@ -2124,7 +2118,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="14">
-        <v>20001255</v>
+        <v>21084321</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>128</v>
@@ -2171,7 +2165,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="14">
-        <v>20001235</v>
+        <v>20011235</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>78</v>
@@ -2218,7 +2212,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="14">
-        <v>20001235</v>
+        <v>20011235</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>78</v>
@@ -2265,7 +2259,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="14">
-        <v>20001237</v>
+        <v>20011237</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>91</v>
@@ -2312,7 +2306,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="14">
-        <v>20001237</v>
+        <v>20011237</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>91</v>
@@ -2359,7 +2353,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="14">
-        <v>20001234</v>
+        <v>20011235</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>100</v>
@@ -2406,7 +2400,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="14">
-        <v>20001234</v>
+        <v>20011235</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>100</v>

</xml_diff>